<commit_message>
Add: Negative Reports, Fix: Negative Reports
</commit_message>
<xml_diff>
--- a/provider/reports/reporte_test_6-1-2024.xlsx
+++ b/provider/reports/reporte_test_6-1-2024.xlsx
@@ -4,6 +4,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="DIA" sheetId="1" r:id="rId1"/>
+    <sheet name="ABONOS" sheetId="2" r:id="rId2"/>
+    <sheet name="SALDOS" sheetId="3" r:id="rId3"/>
+    <sheet name="GASTOS" sheetId="4" r:id="rId4"/>
+    <sheet name="CUENTAS SEMANA" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -398,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -440,7 +444,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve">27/12/2023 </v>
+        <v xml:space="preserve">5/1/2024 </v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -458,10 +462,10 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>600.00</v>
+        <v>100.00</v>
       </c>
       <c r="H2" t="str">
-        <v>169400.00</v>
+        <v>169900.00</v>
       </c>
       <c r="I2" t="str">
         <v>abono</v>
@@ -470,33 +474,33 @@
         <v>nequi</v>
       </c>
       <c r="K2" t="str">
-        <v xml:space="preserve">27/12/2023 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v xml:space="preserve">27/12/2023 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1">
-        <v>45291.999814814815</v>
+        <v>45294.999814814815</v>
       </c>
       <c r="D3" t="str">
-        <v>170000.00</v>
+        <v>123456.00</v>
       </c>
       <c r="E3" t="str">
-        <v>500.00</v>
+        <v>123.00</v>
       </c>
       <c r="F3" t="str">
         <v>0.00</v>
       </c>
       <c r="G3" t="str">
-        <v>600.00</v>
+        <v>123.00</v>
       </c>
       <c r="H3" t="str">
-        <v>169400.00</v>
+        <v>123333.00</v>
       </c>
       <c r="I3" t="str">
         <v>abono</v>
@@ -505,39 +509,39 @@
         <v>nequi</v>
       </c>
       <c r="K3" t="str">
-        <v xml:space="preserve">26/12/2023 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v xml:space="preserve">5/1/2024 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1">
-        <v>45291.999814814815</v>
+        <v>45294.999814814815</v>
       </c>
       <c r="D4" t="str">
-        <v>170000.00</v>
+        <v>123456.00</v>
       </c>
       <c r="E4" t="str">
-        <v>100.00</v>
+        <v>123.00</v>
       </c>
       <c r="F4" t="str">
         <v>0.00</v>
       </c>
       <c r="G4" t="str">
-        <v>700.00</v>
+        <v>492.00</v>
       </c>
       <c r="H4" t="str">
-        <v>169300.00</v>
+        <v>122964.00</v>
       </c>
       <c r="I4" t="str">
         <v>abono</v>
       </c>
       <c r="J4" t="str">
-        <v>nequi</v>
+        <v>efectivo</v>
       </c>
       <c r="K4" t="str">
         <v xml:space="preserve">4/1/2024 </v>
@@ -545,72 +549,72 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v xml:space="preserve">26/12/2023 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1">
-        <v>45285.999814814815</v>
+        <v>45294.999814814815</v>
       </c>
       <c r="D5" t="str">
-        <v>179999.00</v>
+        <v>123456.00</v>
       </c>
       <c r="E5" t="str">
-        <v>120000.00</v>
+        <v>123.00</v>
       </c>
       <c r="F5" t="str">
         <v>0.00</v>
       </c>
       <c r="G5" t="str">
-        <v>120000.00</v>
+        <v>492.00</v>
       </c>
       <c r="H5" t="str">
-        <v>59999.00</v>
+        <v>122964.00</v>
       </c>
       <c r="I5" t="str">
         <v>abono</v>
       </c>
       <c r="J5" t="str">
-        <v>daviplata</v>
+        <v>efectivo</v>
       </c>
       <c r="K5" t="str">
-        <v xml:space="preserve">27/12/2023 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v xml:space="preserve">27/12/2023 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>45285.999814814815</v>
+        <v>45294.999814814815</v>
       </c>
       <c r="D6" t="str">
-        <v>179999.00</v>
+        <v>123456.00</v>
       </c>
       <c r="E6" t="str">
-        <v>200.00</v>
+        <v>123.00</v>
       </c>
       <c r="F6" t="str">
         <v>0.00</v>
       </c>
       <c r="G6" t="str">
-        <v>120200.00</v>
+        <v>492.00</v>
       </c>
       <c r="H6" t="str">
-        <v>59799.00</v>
+        <v>122964.00</v>
       </c>
       <c r="I6" t="str">
         <v>abono</v>
       </c>
       <c r="J6" t="str">
-        <v>nequi</v>
+        <v>efectivo</v>
       </c>
       <c r="K6" t="str">
-        <v xml:space="preserve">26/12/2023 </v>
+        <v xml:space="preserve">4/1/2024 </v>
       </c>
     </row>
     <row r="7">
@@ -618,7 +622,7 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1">
         <v>45294.999814814815</v>
@@ -633,16 +637,16 @@
         <v>0.00</v>
       </c>
       <c r="G7" t="str">
-        <v>123.00</v>
+        <v>492.00</v>
       </c>
       <c r="H7" t="str">
-        <v>123333.00</v>
+        <v>122964.00</v>
       </c>
       <c r="I7" t="str">
         <v>abono</v>
       </c>
       <c r="J7" t="str">
-        <v>nequi</v>
+        <v>efectivo</v>
       </c>
       <c r="K7" t="str">
         <v xml:space="preserve">4/1/2024 </v>
@@ -653,31 +657,31 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1">
         <v>45294.999814814815</v>
       </c>
       <c r="D8" t="str">
-        <v>123456.00</v>
+        <v>1234.00</v>
       </c>
       <c r="E8" t="str">
-        <v>123.00</v>
+        <v>321.00</v>
       </c>
       <c r="F8" t="str">
         <v>0.00</v>
       </c>
       <c r="G8" t="str">
-        <v>492.00</v>
+        <v>321.00</v>
       </c>
       <c r="H8" t="str">
-        <v>122964.00</v>
+        <v>913.00</v>
       </c>
       <c r="I8" t="str">
         <v>abono</v>
       </c>
       <c r="J8" t="str">
-        <v>efectivo</v>
+        <v>tarjeta</v>
       </c>
       <c r="K8" t="str">
         <v xml:space="preserve">4/1/2024 </v>
@@ -688,13 +692,13 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B9">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1">
         <v>45294.999814814815</v>
       </c>
       <c r="D9" t="str">
-        <v>123456.00</v>
+        <v>1234.00</v>
       </c>
       <c r="E9" t="str">
         <v>123.00</v>
@@ -703,16 +707,16 @@
         <v>0.00</v>
       </c>
       <c r="G9" t="str">
-        <v>492.00</v>
+        <v>246.00</v>
       </c>
       <c r="H9" t="str">
-        <v>122964.00</v>
+        <v>988.00</v>
       </c>
       <c r="I9" t="str">
         <v>abono</v>
       </c>
       <c r="J9" t="str">
-        <v>efectivo</v>
+        <v>daviplata</v>
       </c>
       <c r="K9" t="str">
         <v xml:space="preserve">4/1/2024 </v>
@@ -723,13 +727,13 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>45294.999814814815</v>
       </c>
       <c r="D10" t="str">
-        <v>123456.00</v>
+        <v>1234.00</v>
       </c>
       <c r="E10" t="str">
         <v>123.00</v>
@@ -738,16 +742,16 @@
         <v>0.00</v>
       </c>
       <c r="G10" t="str">
-        <v>492.00</v>
+        <v>246.00</v>
       </c>
       <c r="H10" t="str">
-        <v>122964.00</v>
+        <v>988.00</v>
       </c>
       <c r="I10" t="str">
         <v>abono</v>
       </c>
       <c r="J10" t="str">
-        <v>efectivo</v>
+        <v>daviplata</v>
       </c>
       <c r="K10" t="str">
         <v xml:space="preserve">4/1/2024 </v>
@@ -758,25 +762,25 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B11">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1">
         <v>45294.999814814815</v>
       </c>
       <c r="D11" t="str">
-        <v>123456.00</v>
+        <v>1234.00</v>
       </c>
       <c r="E11" t="str">
-        <v>123.00</v>
+        <v>456.00</v>
       </c>
       <c r="F11" t="str">
         <v>0.00</v>
       </c>
       <c r="G11" t="str">
-        <v>492.00</v>
+        <v>456.00</v>
       </c>
       <c r="H11" t="str">
-        <v>122964.00</v>
+        <v>778.00</v>
       </c>
       <c r="I11" t="str">
         <v>abono</v>
@@ -790,37 +794,402 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
+        <v xml:space="preserve">6/1/2024 </v>
       </c>
       <c r="B12">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45296.999814814815</v>
+      </c>
+      <c r="D12" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="E12" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F12" t="str">
+        <v>321.00</v>
+      </c>
+      <c r="G12" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H12" t="str">
+        <v>913.00</v>
+      </c>
+      <c r="I12" t="str">
+        <v>saldo</v>
+      </c>
+      <c r="J12" t="str">
+        <v>efectivo</v>
+      </c>
+      <c r="K12" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B13">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45294.999814814815</v>
+      </c>
+      <c r="D13" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="E13" t="str">
+        <v>12.00</v>
+      </c>
+      <c r="F13" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G13" t="str">
+        <v>12.00</v>
+      </c>
+      <c r="H13" t="str">
+        <v>1222.00</v>
+      </c>
+      <c r="I13" t="str">
+        <v>abono</v>
+      </c>
+      <c r="J13" t="str">
+        <v>nequi</v>
+      </c>
+      <c r="K13" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B14">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45294.999814814815</v>
+      </c>
+      <c r="D14" t="str">
+        <v>200000.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>50000.00</v>
+      </c>
+      <c r="F14" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G14" t="str">
+        <v>50000.00</v>
+      </c>
+      <c r="H14" t="str">
+        <v>150000.00</v>
+      </c>
+      <c r="I14" t="str">
+        <v>abono</v>
+      </c>
+      <c r="J14" t="str">
+        <v>nequi</v>
+      </c>
+      <c r="K14" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B15">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45294.999814814815</v>
+      </c>
+      <c r="D15" t="str">
+        <v>200000.00</v>
+      </c>
+      <c r="E15" t="str">
+        <v>1000.00</v>
+      </c>
+      <c r="F15" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G15" t="str">
+        <v>1000.00</v>
+      </c>
+      <c r="H15" t="str">
+        <v>199000.00</v>
+      </c>
+      <c r="I15" t="str">
+        <v>abono</v>
+      </c>
+      <c r="J15" t="str">
+        <v>nequi</v>
+      </c>
+      <c r="K15" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:K15"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>FechadPago</v>
+      </c>
+      <c r="B1" t="str">
+        <v>IdOrdenCompra</v>
+      </c>
+      <c r="C1" t="str">
+        <v>total_alquiler</v>
+      </c>
+      <c r="D1" t="str">
+        <v>ABONO</v>
+      </c>
+      <c r="E1" t="str">
+        <v>SALDO</v>
+      </c>
+      <c r="F1" t="str">
+        <v>PendientePorPagar</v>
+      </c>
+      <c r="G1" t="str">
+        <v>ABONO_TOTAL</v>
+      </c>
+      <c r="H1" t="str">
+        <v>SALDO_TOTAL</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v xml:space="preserve">5/1/2024 </v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <v>170000.00</v>
+      </c>
+      <c r="D2" t="str">
+        <v>100.00</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F2" t="str">
+        <v>169900.00</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B3">
+        <v>31</v>
+      </c>
+      <c r="C3" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D3" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F3" t="str">
+        <v>123333.00</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D4" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F4" t="str">
+        <v>122964.00</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D5" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F5" t="str">
+        <v>122964.00</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D6" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F6" t="str">
+        <v>122964.00</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D7" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F7" t="str">
+        <v>122964.00</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B8">
         <v>33</v>
       </c>
-      <c r="C12" s="1">
-        <v>45294.999814814815</v>
+      <c r="C8" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D8" t="str">
+        <v>321.00</v>
+      </c>
+      <c r="E8" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F8" t="str">
+        <v>913.00</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B9">
+        <v>34</v>
+      </c>
+      <c r="C9" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D9" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F9" t="str">
+        <v>988.00</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B10">
+        <v>34</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D10" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E10" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F10" t="str">
+        <v>988.00</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B11">
+        <v>36</v>
+      </c>
+      <c r="C11" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D11" t="str">
+        <v>456.00</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F11" t="str">
+        <v>778.00</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v xml:space="preserve">6/1/2024 </v>
+      </c>
+      <c r="B12">
+        <v>37</v>
+      </c>
+      <c r="C12" t="str">
+        <v>1234.00</v>
       </c>
       <c r="D12" t="str">
-        <v>1234.00</v>
+        <v>0.00</v>
       </c>
       <c r="E12" t="str">
         <v>321.00</v>
       </c>
       <c r="F12" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="G12" t="str">
-        <v>321.00</v>
-      </c>
-      <c r="H12" t="str">
         <v>913.00</v>
-      </c>
-      <c r="I12" t="str">
-        <v>abono</v>
-      </c>
-      <c r="J12" t="str">
-        <v>tarjeta</v>
-      </c>
-      <c r="K12" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
       </c>
     </row>
     <row r="13">
@@ -828,34 +1197,19 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B13">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1">
-        <v>45294.999814814815</v>
+        <v>39</v>
+      </c>
+      <c r="C13" t="str">
+        <v>1234.00</v>
       </c>
       <c r="D13" t="str">
-        <v>1234.00</v>
+        <v>12.00</v>
       </c>
       <c r="E13" t="str">
-        <v>123.00</v>
+        <v>0.00</v>
       </c>
       <c r="F13" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="G13" t="str">
-        <v>246.00</v>
-      </c>
-      <c r="H13" t="str">
-        <v>988.00</v>
-      </c>
-      <c r="I13" t="str">
-        <v>abono</v>
-      </c>
-      <c r="J13" t="str">
-        <v>daviplata</v>
-      </c>
-      <c r="K13" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
+        <v>1222.00</v>
       </c>
     </row>
     <row r="14">
@@ -863,34 +1217,19 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B14">
-        <v>34</v>
-      </c>
-      <c r="C14" s="1">
-        <v>45294.999814814815</v>
+        <v>42</v>
+      </c>
+      <c r="C14" t="str">
+        <v>200000.00</v>
       </c>
       <c r="D14" t="str">
-        <v>1234.00</v>
+        <v>50000.00</v>
       </c>
       <c r="E14" t="str">
-        <v>123.00</v>
+        <v>0.00</v>
       </c>
       <c r="F14" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="G14" t="str">
-        <v>246.00</v>
-      </c>
-      <c r="H14" t="str">
-        <v>988.00</v>
-      </c>
-      <c r="I14" t="str">
-        <v>abono</v>
-      </c>
-      <c r="J14" t="str">
-        <v>daviplata</v>
-      </c>
-      <c r="K14" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
+        <v>150000.00</v>
       </c>
     </row>
     <row r="15">
@@ -898,179 +1237,442 @@
         <v xml:space="preserve">4/1/2024 </v>
       </c>
       <c r="B15">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1">
-        <v>45294.999814814815</v>
+        <v>43</v>
+      </c>
+      <c r="C15" t="str">
+        <v>200000.00</v>
       </c>
       <c r="D15" t="str">
-        <v>1234.00</v>
+        <v>1000.00</v>
       </c>
       <c r="E15" t="str">
-        <v>456.00</v>
+        <v>0.00</v>
       </c>
       <c r="F15" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="G15" t="str">
-        <v>456.00</v>
-      </c>
-      <c r="H15" t="str">
-        <v>778.00</v>
-      </c>
-      <c r="I15" t="str">
-        <v>abono</v>
-      </c>
-      <c r="J15" t="str">
-        <v>efectivo</v>
-      </c>
-      <c r="K15" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
+        <v>199000.00</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
-        <v xml:space="preserve">6/1/2024 </v>
-      </c>
-      <c r="B16">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1">
-        <v>45296.999814814815</v>
-      </c>
-      <c r="D16" t="str">
-        <v>1234.00</v>
-      </c>
-      <c r="E16" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
+        <v>52750.00</v>
+      </c>
+      <c r="H16" t="str">
         <v>321.00</v>
-      </c>
-      <c r="G16" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="H16" t="str">
-        <v>913.00</v>
-      </c>
-      <c r="I16" t="str">
-        <v>saldo</v>
-      </c>
-      <c r="J16" t="str">
-        <v>efectivo</v>
-      </c>
-      <c r="K16" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
-      </c>
-      <c r="B17">
-        <v>39</v>
-      </c>
-      <c r="C17" s="1">
-        <v>45294.999814814815</v>
-      </c>
-      <c r="D17" t="str">
-        <v>1234.00</v>
-      </c>
-      <c r="E17" t="str">
-        <v>12.00</v>
-      </c>
-      <c r="F17" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="G17" t="str">
-        <v>12.00</v>
-      </c>
-      <c r="H17" t="str">
-        <v>1222.00</v>
-      </c>
-      <c r="I17" t="str">
-        <v>abono</v>
-      </c>
-      <c r="J17" t="str">
-        <v>nequi</v>
-      </c>
-      <c r="K17" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
-      </c>
-      <c r="B18">
-        <v>42</v>
-      </c>
-      <c r="C18" s="1">
-        <v>45294.999814814815</v>
-      </c>
-      <c r="D18" t="str">
-        <v>200000.00</v>
-      </c>
-      <c r="E18" t="str">
-        <v>50000.00</v>
-      </c>
-      <c r="F18" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="G18" t="str">
-        <v>50000.00</v>
-      </c>
-      <c r="H18" t="str">
-        <v>150000.00</v>
-      </c>
-      <c r="I18" t="str">
-        <v>abono</v>
-      </c>
-      <c r="J18" t="str">
-        <v>nequi</v>
-      </c>
-      <c r="K18" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
-      </c>
-      <c r="B19">
-        <v>43</v>
-      </c>
-      <c r="C19" s="1">
-        <v>45294.999814814815</v>
-      </c>
-      <c r="D19" t="str">
-        <v>200000.00</v>
-      </c>
-      <c r="E19" t="str">
-        <v>1000.00</v>
-      </c>
-      <c r="F19" t="str">
-        <v>0.00</v>
-      </c>
-      <c r="G19" t="str">
-        <v>1000.00</v>
-      </c>
-      <c r="H19" t="str">
-        <v>199000.00</v>
-      </c>
-      <c r="I19" t="str">
-        <v>abono</v>
-      </c>
-      <c r="J19" t="str">
-        <v>nequi</v>
-      </c>
-      <c r="K19" t="str">
-        <v xml:space="preserve">4/1/2024 </v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>FechadPago</v>
+      </c>
+      <c r="B1" t="str">
+        <v>IdOrdenCompra</v>
+      </c>
+      <c r="C1" t="str">
+        <v>total_alquiler</v>
+      </c>
+      <c r="D1" t="str">
+        <v>ABONO</v>
+      </c>
+      <c r="E1" t="str">
+        <v>SALDO</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B2">
+        <v>31</v>
+      </c>
+      <c r="C2" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D2" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E2" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D3" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E3" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D4" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D5" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6" t="str">
+        <v>123456.00</v>
+      </c>
+      <c r="D6" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B7">
+        <v>33</v>
+      </c>
+      <c r="C7" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D7" t="str">
+        <v>321.00</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D8" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E8" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B9">
+        <v>34</v>
+      </c>
+      <c r="C9" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D9" t="str">
+        <v>123.00</v>
+      </c>
+      <c r="E9" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B10">
+        <v>36</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D10" t="str">
+        <v>456.00</v>
+      </c>
+      <c r="E10" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B11">
+        <v>39</v>
+      </c>
+      <c r="C11" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D11" t="str">
+        <v>12.00</v>
+      </c>
+      <c r="E11" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v xml:space="preserve">5/1/2024 </v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="str">
+        <v>170000.00</v>
+      </c>
+      <c r="D12" t="str">
+        <v>100.00</v>
+      </c>
+      <c r="E12" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B13">
+        <v>42</v>
+      </c>
+      <c r="C13" t="str">
+        <v>200000.00</v>
+      </c>
+      <c r="D13" t="str">
+        <v>50000.00</v>
+      </c>
+      <c r="E13" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v xml:space="preserve">4/1/2024 </v>
+      </c>
+      <c r="B14">
+        <v>43</v>
+      </c>
+      <c r="C14" t="str">
+        <v>200000.00</v>
+      </c>
+      <c r="D14" t="str">
+        <v>1000.00</v>
+      </c>
+      <c r="E14" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v xml:space="preserve">6/1/2024 </v>
+      </c>
+      <c r="B15">
+        <v>37</v>
+      </c>
+      <c r="C15" t="str">
+        <v>1234.00</v>
+      </c>
+      <c r="D15" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="E15" t="str">
+        <v>321.00</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E15"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>SALDO_TOTAL</v>
+      </c>
+      <c r="B1" t="str">
+        <v>ABONO_TOTAL</v>
+      </c>
+      <c r="C1" t="str">
+        <v>IdTipoPago</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Descripcion</v>
+      </c>
+      <c r="E1" t="str">
+        <v>TotalPagosNequi</v>
+      </c>
+      <c r="F1" t="str">
+        <v>TotalSumaDaviplata</v>
+      </c>
+      <c r="G1" t="str">
+        <v>PagoTotalEfectivo</v>
+      </c>
+      <c r="H1" t="str">
+        <v>PagoTotalTarjeta</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>321.00</v>
+      </c>
+      <c r="B2" t="str">
+        <v>52750.00</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>nequi</v>
+      </c>
+      <c r="E3" t="str">
+        <v>51235.00</v>
+      </c>
+      <c r="F3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G3" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H3" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>daviplata</v>
+      </c>
+      <c r="E4" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F4" t="str">
+        <v>246.00</v>
+      </c>
+      <c r="G4" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H4" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="str">
+        <v>efectivo</v>
+      </c>
+      <c r="E5" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F5" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G5" t="str">
+        <v>1269.00</v>
+      </c>
+      <c r="H5" t="str">
+        <v>0.00</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="str">
+        <v>tarjeta</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="F6" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="G6" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="H6" t="str">
+        <v>321.00</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>